<commit_message>
Added new forms details
</commit_message>
<xml_diff>
--- a/backend/exports/SPARS_Excel_DB.xlsx
+++ b/backend/exports/SPARS_Excel_DB.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Newsletter Subscriptions" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Contact Forms" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Brochure Requests" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Product Profile Requests" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Talk to Sales" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Newsletter Subscriptions" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contact Forms" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Brochure Requests" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Product Profile Requests" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Talk to Sales" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -471,13 +471,13 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-11-28 14:41:57</t>
+          <t>2026-01-23 11:33:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -486,13 +486,13 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-11-28 11:46:25</t>
+          <t>2026-01-23 11:29:58</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -501,13 +501,13 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-11-28 11:43:01</t>
+          <t>2026-01-23 11:29:47</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -516,28 +516,28 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-11-28 10:47:27</t>
+          <t>2026-01-23 11:28:50</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ra147001y@gmail.com</t>
+          <t>test@example.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-11-28 10:18:05</t>
+          <t>2026-01-23 11:22:27</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -546,13 +546,13 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-11-27 15:30:00</t>
+          <t>2025-11-28 14:41:57</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -561,13 +561,13 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-11-27 15:24:40</t>
+          <t>2025-11-28 11:46:25</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -576,13 +576,13 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-11-27 15:14:45</t>
+          <t>2025-11-28 11:43:01</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -591,35 +591,110 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-11-27 07:33:55</t>
+          <t>2025-11-28 10:47:27</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>ra147001y@gmail.com</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-11-27 06:46:18</t>
+          <t>2025-11-28 10:18:05</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-11-27 15:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-11-27 15:24:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-11-27 15:14:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-11-27 07:33:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-11-27 06:46:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
         <v>1</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>2025-11-27 06:44:40</t>
         </is>
@@ -636,7 +711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -648,9 +723,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="31" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="19" customWidth="1" min="5" max="5"/>
     <col width="42" customWidth="1" min="6" max="6"/>
-    <col width="9" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="21" customWidth="1" min="9" max="9"/>
   </cols>
@@ -704,143 +779,147 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>m</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Azhar</t>
+          <t>Yaqoob</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>azharawanss355@gmail.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0345856455</t>
+          <t>+1 (555) 123-4567</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>az_tech</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
+          <t>Test Business Inc.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>This is a test demo request from the automated testing script. Please ignore.</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2026-01-21 04:33:32</t>
+          <t>2026-01-23 11:30:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Azhar</t>
+          <t>Yaqoob</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>azhar@vcs.com.pk</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0345856455</t>
+          <t>+1 (555) 123-4567</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>az_tech</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2026-01-22</t>
-        </is>
-      </c>
+          <t>Test Business Inc.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>This is a test message from the automated form testing script. Please ignore this email.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2026-01-21 04:32:22</t>
+          <t>2026-01-23 11:30:01</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rizwan</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mahmood</t>
+          <t>Yaqoob</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>rizwan@vcs.com.pk</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>+923318406191</t>
+          <t>+1 (555) 123-4567</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Visionary Computer Solutions (Pvt.) Ltd.</t>
+          <t>Test Business Inc.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>testing</t>
+          <t>This is a test demo request from the automated testing script. Please ignore.</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2026-01-21 04:02:34</t>
+          <t>2026-01-23 11:29:31</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>sdfsd</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>sdfsd</t>
+          <t>Yaqoob</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -850,103 +929,312 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2424242424</t>
+          <t>+1 (555) 123-4567</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ghgh</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2026-01-21</t>
-        </is>
-      </c>
+          <t>Test Business Inc.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>This is a test message from the automated form testing script. Please ignore this email.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2026-01-20 00:22:20</t>
+          <t>2026-01-23 11:29:23</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ahmed</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Yaqoob</t>
+          <t>User</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>test@example.com</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>03147261655</t>
+          <t>1234567890</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>VCS</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2025-12-19</t>
-        </is>
-      </c>
+          <t>Test Company</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>This is a test message</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2025-12-02 02:26:32</t>
+          <t>2026-01-23 11:22:29</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ahmed</t>
+          <t>m</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Yaqoob</t>
+          <t>Azhar</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>azharawanss355@gmail.com</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>03147261655</t>
+          <t>0345856455</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>VCS</t>
+          <t>az_tech</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2026-01-21 04:33:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Azhar</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>azhar@vcs.com.pk</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0345856455</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>az_tech</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2026-01-21 04:32:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Rizwan</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Mahmood</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>rizwan@vcs.com.pk</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>+923318406191</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Visionary Computer Solutions (Pvt.) Ltd.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2026-01-22</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2026-01-21 04:02:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sdfsd</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>sdfsd</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2424242424</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ghgh</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2026-01-21</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2026-01-20 00:22:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Ahmed</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Yaqoob</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2025-12-19</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2025-12-02 02:26:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Ahmed</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Yaqoob</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>2025-11-30</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>2025-11-27 07:38:20</t>
         </is>
@@ -963,7 +1251,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -974,9 +1262,9 @@
     <col width="4" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="31" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="31" customWidth="1" min="4" max="4"/>
+    <col width="19" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
   </cols>
@@ -1025,21 +1313,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ahmedyaqoob</t>
+          <t>rhtr</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ra147001y@gmail.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>23er32rf</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1051,31 +1339,39 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-01-21 04:26:17</t>
+          <t>2026-01-23 11:35:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dsfsdf</t>
+          <t>Ahmed Yaqoob</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ahmedyaqoobusiness@gmail.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sdfdsfdsf</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+          <t>Test Business Inc.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>+1 (555) 123-4567</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Operations Manager</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1083,17 +1379,17 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2026-01-21 04:24:08</t>
+          <t>2026-01-23 11:30:03</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>adsfas</t>
+          <t>Ahmed Yaqoob</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1103,15 +1399,19 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>dsfdsf</t>
+          <t>Test Business Inc.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>6615151515</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+          <t>+1 (555) 123-4567</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Operations Manager</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1119,27 +1419,27 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2026-01-21 04:09:04</t>
+          <t>2026-01-23 11:29:25</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ahmed yaqoob</t>
+          <t>ahmedyaqoob</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>ra147001y@gmail.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>VCS</t>
+          <t>23er32rf</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1151,27 +1451,27 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2026-01-21 02:34:14</t>
+          <t>2026-01-21 04:26:17</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>gfg</t>
+          <t>dsfsdf</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ra147001y@gmail.com</t>
+          <t>ahmedyaqoobusiness@gmail.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>asdfdasf</t>
+          <t>sdfdsfdsf</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1183,17 +1483,17 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2026-01-20 00:20:13</t>
+          <t>2026-01-21 04:24:08</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ahmed Yaqoob</t>
+          <t>adsfas</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1203,10 +1503,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>VCS</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>dsfdsf</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>6615151515</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
@@ -1215,22 +1519,22 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-11-28 15:55:52</t>
+          <t>2026-01-21 04:09:04</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ahmed Yaqoob</t>
+          <t>ahmed yaqoob</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ra147001y@gmail.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1247,27 +1551,27 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-11-28 15:30:00</t>
+          <t>2026-01-21 02:34:14</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ahmed Yaqoob</t>
+          <t>gfg</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>ra147001y@gmail.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>VCS</t>
+          <t>asdfdasf</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -1279,17 +1583,17 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-11-28 11:51:54</t>
+          <t>2026-01-20 00:20:13</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ahmed</t>
+          <t>Ahmed Yaqoob</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1311,22 +1615,22 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-11-27 15:53:43</t>
+          <t>2025-11-28 15:55:52</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ahmed</t>
+          <t>Ahmed Yaqoob</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>ra147001y@gmail.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1343,17 +1647,17 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-11-27 15:35:09</t>
+          <t>2025-11-28 15:30:00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ahmed</t>
+          <t>Ahmed Yaqoob</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1375,17 +1679,17 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-11-27 15:33:13</t>
+          <t>2025-11-28 11:51:54</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ahmed Yaqoob</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1407,17 +1711,17 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-11-27 07:31:09</t>
+          <t>2025-11-27 15:53:43</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ahmed Yaqoob</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1439,17 +1743,17 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-11-27 07:08:24</t>
+          <t>2025-11-27 15:35:09</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Ahmed Yaqoob</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1471,13 +1775,13 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-11-27 07:06:38</t>
+          <t>2025-11-27 15:33:13</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1503,22 +1807,22 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-11-27 07:03:19</t>
+          <t>2025-11-27 07:31:09</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ahmed yaqoob</t>
+          <t>Ahmed Yaqoob</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbbusiness@gmai.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1535,22 +1839,22 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-11-27 06:49:51</t>
+          <t>2025-11-27 07:08:24</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Ahmed yaqoob</t>
+          <t>Ahmed Yaqoob</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbbusiness@gmai.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1567,22 +1871,22 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-11-27 06:49:17</t>
+          <t>2025-11-27 07:06:38</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Ahmed yaqoob</t>
+          <t>Ahmed Yaqoob</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbbusiness@gmai.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1599,13 +1903,13 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-11-27 06:48:29</t>
+          <t>2025-11-27 07:03:19</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1630,6 +1934,102 @@
         </is>
       </c>
       <c r="H20" t="inlineStr">
+        <is>
+          <t>2025-11-27 06:49:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ahmed yaqoob</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbbusiness@gmai.com</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2025-11-27 06:49:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Ahmed yaqoob</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbbusiness@gmai.com</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2025-11-27 06:48:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ahmed yaqoob</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbbusiness@gmai.com</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
         <is>
           <t>2025-11-27 06:48:02</t>
         </is>
@@ -1646,7 +2046,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1658,18 +2058,18 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="31" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="10" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
-    <col width="9" customWidth="1" min="10" max="10"/>
-    <col width="9" customWidth="1" min="11" max="11"/>
-    <col width="16" customWidth="1" min="12" max="12"/>
+    <col width="19" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="17" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="37" customWidth="1" min="11" max="11"/>
+    <col width="26" customWidth="1" min="12" max="12"/>
     <col width="12" customWidth="1" min="13" max="13"/>
     <col width="7" customWidth="1" min="14" max="14"/>
-    <col width="14" customWidth="1" min="15" max="15"/>
-    <col width="10" customWidth="1" min="16" max="16"/>
+    <col width="50" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
     <col width="21" customWidth="1" min="17" max="17"/>
   </cols>
   <sheetData>
@@ -1762,16 +2162,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dsfsdf</t>
+          <t>jhjhk</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>jhkj</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1781,13 +2181,13 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>45454545</t>
+          <t>5725742</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>dsfdsf</t>
+          <t>275</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -1801,22 +2201,22 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2026-01-21 04:27:48</t>
+          <t>2026-01-23 11:37:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>sfds</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>Yaqoob</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1826,87 +2226,159 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>54545454545</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>+1 (555) 123-4567</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Operations Manager</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>sdfsdfsdf</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+          <t>Test Business Inc.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Home Furnishing</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>51-200 employees</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>https://www.testbusiness.com</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>123 Test Street, New York, NY 10001</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Excel &amp; Manual Processes</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" t="n">
+        <v>25</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Need comprehensive ERP solution for inventory and order management</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>3-6 months</t>
+        </is>
+      </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2026-01-20 00:21:21</t>
+          <t>2026-01-23 11:30:05</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>adf</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>sdfa</t>
+          <t>Yaqoob</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ahmeds@am.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>021205202052</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+          <t>+1 (555) 123-4567</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Operations Manager</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>fr</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+          <t>Test Business Inc.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Home Furnishing</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>51-200 employees</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://www.testbusiness.com</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>123 Test Street, New York, NY 10001</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Excel &amp; Manual Processes</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" t="n">
+        <v>25</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Need comprehensive ERP solution for inventory and order management</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>3-6 months</t>
+        </is>
+      </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-11-28 15:38:09</t>
+          <t>2026-01-23 11:29:27</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ahmed</t>
+          <t>dsfsdf</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Yaqoob</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1916,13 +2388,13 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>03147261655</t>
+          <t>45454545</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>VCS</t>
+          <t>dsfdsf</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -1936,22 +2408,22 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-11-27 07:13:55</t>
+          <t>2026-01-21 04:27:48</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ahmed </t>
+          <t>sfds</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Yaqoob</t>
+          <t>sdfdsf</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1961,13 +2433,13 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>03147261655</t>
+          <t>54545454545</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>VCS</t>
+          <t>sdfsdfsdf</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -1981,38 +2453,38 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-11-27 06:54:19</t>
+          <t>2026-01-20 00:21:21</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ahmed </t>
+          <t>adf</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Yaqoob</t>
+          <t>sdfa</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>ahmeds@am.com</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>03147261655</t>
+          <t>021205202052</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>VCS</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
@@ -2026,17 +2498,17 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-11-27 06:50:58</t>
+          <t>2025-11-28 15:38:09</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ahmed </t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2070,6 +2542,141 @@
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
+        <is>
+          <t>2025-11-27 07:13:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ahmed </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Yaqoob</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>2025-11-27 06:54:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ahmed </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Yaqoob</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>2025-11-27 06:50:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ahmed </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Yaqoob</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr">
         <is>
           <t>2025-11-27 06:50:43</t>
         </is>
@@ -2086,7 +2693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2097,9 +2704,9 @@
     <col width="4" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="31" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="9" customWidth="1" min="5" max="5"/>
-    <col width="29" customWidth="1" min="6" max="6"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -2142,46 +2749,42 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>azhar</t>
+          <t>geg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>azhar@vcs.com.pk</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0345856455</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>az_tech</t>
-        </is>
-      </c>
+          <t>5725742</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>hello</t>
+          <t>4\1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2026-01-21 04:35:17</t>
+          <t>2026-01-23 11:38:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>sdfdsfds</t>
+          <t>Ahmed Yaqoob</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2191,125 +2794,137 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5656565656</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>+1 (555) 123-4567</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Test Business Inc.</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>565</t>
+          <t>I'm interested in learning more about SPARS ERP solution. Please contact me to schedule a demo.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2026-01-20 00:23:12</t>
+          <t>2026-01-23 11:30:07</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ahmed</t>
+          <t>Ahmed Yaqoob</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>i201865@nu.edu.pk</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>03147261655</t>
+          <t>+1 (555) 123-4567</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>VCS</t>
+          <t>Test Business Inc.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>SIUUUUUUUUUUUUU</t>
+          <t>I'm interested in learning more about SPARS ERP solution. Please contact me to schedule a demo.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-12-04 02:10:50</t>
+          <t>2026-01-23 11:29:29</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ahmed Yaqoob</t>
+          <t>Test User</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>test@example.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>03147261655</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Test Company</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>I am testing it.</t>
+          <t>I want to learn more about SPARS</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-11-27 07:36:11</t>
+          <t>2026-01-23 11:22:31</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ahmed Yaqoob</t>
+          <t>azhar</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>azhar@vcs.com.pk</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>03147261655</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>0345856455</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>az_tech</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Testing</t>
+          <t>hello</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-11-27 06:53:09</t>
+          <t>2026-01-21 04:35:17</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ahmed Yaqoob</t>
+          <t>sdfdsfds</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2319,16 +2934,144 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>03147261655</t>
+          <t>5656565656</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2026-01-20 00:23:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ahmed</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>i201865@nu.edu.pk</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>SIUUUUUUUUUUUUU</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025-12-04 02:10:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ahmed Yaqoob</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>I am testing it.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2025-11-27 07:36:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Ahmed Yaqoob</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-11-27 06:53:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Ahmed Yaqoob</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>Talk to Sales form testing.</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>2025-11-27 06:52:09</t>
         </is>

</xml_diff>

<commit_message>
Updated the email services
</commit_message>
<xml_diff>
--- a/backend/exports/SPARS_Excel_DB.xlsx
+++ b/backend/exports/SPARS_Excel_DB.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,127 +463,127 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ahmedyaqobbusiness@gmail.com</t>
+          <t>ra147001y@gmail.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2026-01-23 12:05:31</t>
+          <t>2026-01-26 21:26:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>rizwan@vcs.com.pk</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2026-01-23 11:05:22</t>
+          <t>2026-01-26 01:45:04</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>hassanrasool1057@gmail.com</t>
+          <t>ahmedyaqobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2026-01-23 11:04:36</t>
+          <t>2026-01-23 12:05:31</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>rizwan@vcs.com.pk</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2026-01-23 07:37:49</t>
+          <t>2026-01-23 11:05:22</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ra147001y@gmail.com</t>
+          <t>hassanrasool1057@gmail.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2026-01-23 07:02:03</t>
+          <t>2026-01-23 11:04:36</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ra147001y@gmail.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2026-01-23 06:56:04</t>
+          <t>2026-01-23 07:37:49</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>ra147001y@gmail.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2026-01-23 06:54:20</t>
+          <t>2026-01-23 07:02:03</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ahmed.yaqoob@snapdev.ai</t>
+          <t>ra147001y@gmail.com</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2026-01-23 06:41:43</t>
+          <t>2026-01-23 06:56:04</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -592,20 +592,50 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2026-01-23 05:38:39</t>
+          <t>2026-01-23 06:54:20</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ahmed.yaqoob@snapdev.ai</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2026-01-23 06:41:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2026-01-23 05:38:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
         <v>1</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>ra147001y@gmail.com</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>2026-01-23 05:06:27</t>
         </is>
@@ -622,7 +652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,10 +663,10 @@
     <col width="4" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="31" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="40" customWidth="1" min="6" max="6"/>
-    <col width="45" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
@@ -684,47 +714,50 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rizwan</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mahmood</t>
+          <t>Mandapati</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>rizwan@vcs.com.pk</t>
+          <t>michael@warpandweft.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>+923318406191</t>
+          <t>2125460944</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Visionary Computer Solutions (Pvt) Ltd</t>
+          <t>Warp &amp; Weft</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Testing General Inquiry Form of sparsus.com</t>
+          <t xml:space="preserve">Hello:  I have been recommended by my CPA, Farid Padela and I'm interested in knowing more about your system. Please call to discuss further.
+Thank you,
+Michael
+</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-01-23 11:19:09</t>
+          <t>2026-01-28 10:37:14</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -743,48 +776,160 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>+923318406191</t>
+          <t>03318406191</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Visionary Computer Solutions (Pvt) Ltd</t>
+          <t>VCS</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Testing of General Inquiry Form</t>
+          <t>Testing of the Message field on General Inquiry Form</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2026-01-23 11:07:28</t>
+          <t>2026-01-26 02:31:40</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>adsfaf</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>Ahmed</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Yaqoob</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ra147001y@gmail.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2026-01-26 01:23:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Rizwan</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Mahmood</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>rizwan@vcs.com.pk</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>+923318406191</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Visionary Computer Solutions (Pvt) Ltd</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Testing General Inquiry Form of sparsus.com</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2026-01-23 11:19:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Rizwan</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Mahmood</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>rizwan@vcs.com.pk</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>+923318406191</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Visionary Computer Solutions (Pvt) Ltd</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Testing of General Inquiry Form</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2026-01-23 11:07:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>adsfaf</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ra147001y@gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>dsf</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>2026-01-23 05:03:11</t>
         </is>
@@ -801,7 +946,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -812,11 +957,11 @@
     <col width="4" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
-    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="31" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="42" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
-    <col width="22" customWidth="1" min="8" max="8"/>
+    <col width="50" customWidth="1" min="8" max="8"/>
     <col width="21" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
@@ -869,7 +1014,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -888,66 +1033,357 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>+923318406191</t>
+          <t>03318406191</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Visionary Computer Solutions (Pvt.) Ltd.</t>
+          <t>VCS</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Testing of Demo Form</t>
+          <t>Testing of Additional Information on Demo Request Form of SPARS Website.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2026-01-23 11:06:49</t>
+          <t>2026-01-26 02:28:33</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>adsfa</t>
+          <t>ahmed</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>adfad</t>
+          <t>yaqoob</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ra147001y@gmail.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>515454541</t>
+          <t>03147261655</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>webzone.pk</t>
+          <t>asdf</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
+        <is>
+          <t>2026-01-26 01:20:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ahmed</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>yaqoob</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0314247610</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>vcs</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2026-01-26 01:15:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ahmed</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>yaqoob</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>vcs</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2026-01-26 01:08:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ahmed</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>yaqoob</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>vcs</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2026-01-29</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2026-01-26 00:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ahmed</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>yaqoob</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>vcsa</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2026-01-25 23:57:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ahmed</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>yaqoob</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>03147261655</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2026-01-25 23:47:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Rizwan</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Mahmood</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>rizwan@vcs.com.pk</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>+923318406191</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Visionary Computer Solutions (Pvt.) Ltd.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2026-01-26</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Testing of Demo Form</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2026-01-23 11:06:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>adsfa</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>adfad</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ra147001y@gmail.com</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>515454541</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>webzone.pk</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2026-01-24</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
         <is>
           <t>2026-01-23 05:05:49</t>
         </is>
@@ -1403,7 +1839,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1412,16 +1848,16 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
     <col width="31" customWidth="1" min="3" max="3"/>
-    <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
     <col width="9" customWidth="1" min="5" max="5"/>
-    <col width="9" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="48" customWidth="1" min="6" max="6"/>
+    <col width="37" customWidth="1" min="7" max="7"/>
     <col width="22" customWidth="1" min="8" max="8"/>
     <col width="26" customWidth="1" min="9" max="9"/>
-    <col width="37" customWidth="1" min="10" max="10"/>
-    <col width="25" customWidth="1" min="11" max="11"/>
+    <col width="50" customWidth="1" min="10" max="10"/>
+    <col width="42" customWidth="1" min="11" max="11"/>
     <col width="21" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
@@ -1489,85 +1925,119 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ahmed</t>
+          <t>Rizwan Mahmood</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ahmedyaqoobbusiness@gmail.com</t>
+          <t>rizwan@vcs.com.pk</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>9588880</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>+923318406191</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>VCS</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Cccc</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+          <t>Testing of Message Field on Talk to Sales Form</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Testing of Current ERP System Field</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>500</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Testing of Specific Requirements or Challenges field</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>testing of Implementation Timeline field</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2026-01-24 03:12:18</t>
+          <t>2026-01-26 02:29:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ahmedyqoob</t>
+          <t>ahmed</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ra147001y@gmail.com</t>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>15151</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>03147260655</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>vcs</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>sdfs</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>SAP</t>
+        </is>
+      </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>10</v>
+      </c>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>6 months</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2026-01-23 05:07:03</t>
+          <t>2026-01-26 01:21:32</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>adfaf</t>
+          <t>Ahmed</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1577,29 +2047,103 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8545454</t>
+          <t>9588880</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>sdfsdf</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>SAP</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>10</v>
-      </c>
+          <t>Cccc</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
+        <is>
+          <t>2026-01-24 03:12:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ahmedyqoob</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ra147001y@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>15151</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>sdfs</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2026-01-23 05:07:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>adfaf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ahmedyaqoobbusiness@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>8545454</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>sdfsdf</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>SAP</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>10</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
         <is>
           <t>2026-01-23 05:00:41</t>
         </is>

</xml_diff>